<commit_message>
basic html/css tags. initial project and items rendering
</commit_message>
<xml_diff>
--- a/doc/app_design.xlsx
+++ b/doc/app_design.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlos/coding/Javascript/JS_ToDo_App/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E2BA0D-F027-714C-BE47-7AA899BAC4D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBD539C-9D08-C84A-B571-FC7D86A6B0C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="-19880" windowWidth="27260" windowHeight="17820" xr2:uid="{CF187F84-17D4-F34A-813B-21E404B78F95}"/>
+    <workbookView xWindow="1440" yWindow="1180" windowWidth="27260" windowHeight="17820" activeTab="1" xr2:uid="{CF187F84-17D4-F34A-813B-21E404B78F95}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="App Screens" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -153,7 +154,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -208,6 +209,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C01BC12-D96A-484D-8DA9-ABBD84A7B4AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="647700" y="8255000"/>
+          <a:ext cx="13538200" cy="6896100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7995CE71-669F-B84A-A850-4E297ABAC9E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="825500" y="812800"/>
+          <a:ext cx="12903200" cy="6921500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -509,48 +603,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D050E151-9666-3E43-B904-74D5E709DCCE}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="3" width="45.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="B7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -558,7 +652,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="B9" t="s">
         <v>27</v>
       </c>
@@ -566,7 +660,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -574,12 +668,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="B14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -590,7 +684,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="B16" t="s">
         <v>7</v>
       </c>
@@ -598,12 +692,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="B18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -611,10 +705,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -622,27 +716,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="B25" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="B26" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="B27" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="B28" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="B29" t="s">
         <v>7</v>
       </c>
@@ -650,32 +744,32 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3">
       <c r="B32" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2">
       <c r="B33" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2">
       <c r="B34" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>32</v>
       </c>
@@ -683,7 +777,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -691,7 +785,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>34</v>
       </c>
@@ -699,7 +793,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>35</v>
       </c>
@@ -707,7 +801,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -718,4 +812,19 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750BC0D7-3AC1-514D-A74F-7C9B7716C08B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="R47" sqref="R47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>